<commit_message>
push pour le rendu de projet
</commit_message>
<xml_diff>
--- a/assets/uploads/triathle Noyon.xlsx
+++ b/assets/uploads/triathle Noyon.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="122">
   <si>
     <t xml:space="preserve">Club</t>
   </si>
@@ -185,6 +185,9 @@
     <t xml:space="preserve">M50</t>
   </si>
   <si>
+    <t xml:space="preserve">1min50</t>
+  </si>
+  <si>
     <t xml:space="preserve">Decouverte</t>
   </si>
   <si>
@@ -291,6 +294,9 @@
   </si>
   <si>
     <t xml:space="preserve">HAMOUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3min00</t>
   </si>
   <si>
     <t xml:space="preserve">LEPARC</t>
@@ -387,10 +393,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="166" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* \-??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00\ _€;\-#,##0.00\ _€"/>
+    <numFmt numFmtId="167" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="168" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -547,7 +555,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -580,6 +588,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -612,7 +628,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -624,11 +640,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -640,7 +656,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -660,7 +676,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -748,22 +764,22 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.71"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -792,7 +808,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -856,7 +872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -888,7 +904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -920,7 +936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
@@ -952,7 +968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
@@ -984,7 +1000,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
@@ -1016,7 +1032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
@@ -1048,7 +1064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
@@ -1080,7 +1096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
@@ -1112,7 +1128,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
@@ -1144,7 +1160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
@@ -1176,7 +1192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
@@ -1222,8 +1238,8 @@
       <c r="E15" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="6" t="n">
-        <v>1.5</v>
+      <c r="F15" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>23</v>
@@ -1243,16 +1259,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
@@ -1268,24 +1284,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>53</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>13</v>
@@ -1300,7 +1316,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
@@ -1311,10 +1327,10 @@
         <v>25</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F18" s="6" t="n">
         <v>1.25</v>
@@ -1332,21 +1348,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
@@ -1362,7 +1378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
@@ -1370,16 +1386,16 @@
         <v>28</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>13</v>
@@ -1394,7 +1410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
@@ -1402,16 +1418,16 @@
         <v>28</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>23</v>
@@ -1426,7 +1442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
@@ -1434,16 +1450,16 @@
         <v>28</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>13</v>
@@ -1458,18 +1474,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>49</v>
@@ -1488,7 +1504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
@@ -1496,13 +1512,13 @@
         <v>24</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F24" s="6" t="n">
         <v>2.55</v>
@@ -1520,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
@@ -1528,16 +1544,16 @@
         <v>28</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>13</v>
@@ -1552,24 +1568,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>13</v>
@@ -1584,7 +1600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
@@ -1595,12 +1611,12 @@
         <v>25</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" s="6" t="n">
+        <v>57</v>
+      </c>
+      <c r="F27" s="9" t="n">
         <v>2.3</v>
       </c>
       <c r="G27" s="6" t="s">
@@ -1616,7 +1632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
@@ -1624,16 +1640,16 @@
         <v>24</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28" s="6" t="n">
-        <v>3</v>
+        <v>67</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>91</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>23</v>
@@ -1648,21 +1664,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+      <c r="B29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
@@ -1670,16 +1700,16 @@
         <v>24</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>13</v>
@@ -1690,25 +1720,23 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>93</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F31" s="3"/>
       <c r="G31" s="3" t="s">
         <v>13</v>
       </c>
@@ -1718,25 +1746,27 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F32" s="3"/>
+        <v>57</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G32" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>50</v>
@@ -1744,27 +1774,25 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>93</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>50</v>
@@ -1772,25 +1800,25 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>50</v>
@@ -1798,7 +1826,7 @@
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
@@ -1806,13 +1834,13 @@
         <v>24</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3" t="s">
@@ -1824,32 +1852,19 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="n">
         <f aca="false">A35+1</f>
         <v>35</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0"/>
+      <c r="E36" s="0"/>
+      <c r="F36" s="0"/>
+      <c r="G36" s="0"/>
+      <c r="H36" s="0"/>
+      <c r="I36" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1873,1071 +1888,1071 @@
       <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8"/>
-      <c r="B1" s="9" t="s">
+    <row r="1" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10"/>
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="E1" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>108</v>
+      <c r="I1" s="13" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="n">
+      <c r="A2" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="15" t="s">
+      <c r="C2" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="16" t="n">
+      <c r="D2" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="18" t="n">
         <v>38185</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>110</v>
+      <c r="F2" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="n">
+      <c r="A3" s="15" t="n">
         <f aca="false">A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="17" t="s">
+      <c r="B3" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17" t="s">
+      <c r="D3" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>110</v>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="n">
+      <c r="A4" s="15" t="n">
         <f aca="false">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="19" t="n">
+      <c r="D4" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="21" t="n">
         <v>37691</v>
       </c>
-      <c r="F4" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="17" t="s">
+      <c r="F4" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>110</v>
+      <c r="H4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="n">
+      <c r="A5" s="15" t="n">
         <f aca="false">A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="15" t="s">
+      <c r="C5" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="16" t="n">
+      <c r="D5" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="18" t="n">
         <v>37340</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="18" t="s">
+      <c r="F5" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="19" t="s">
         <v>111</v>
       </c>
+      <c r="H5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="n">
+      <c r="A6" s="15" t="n">
         <f aca="false">A5+1</f>
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="15" t="s">
+      <c r="C6" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="16" t="n">
+      <c r="D6" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="18" t="n">
         <v>37324</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="18" t="s">
+      <c r="F6" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="19" t="s">
         <v>111</v>
       </c>
+      <c r="H6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="n">
+      <c r="A7" s="15" t="n">
         <f aca="false">A6+1</f>
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="C7" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>111</v>
+      <c r="D7" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="n">
+      <c r="A8" s="15" t="n">
         <f aca="false">A7+1</f>
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="17" t="s">
+      <c r="C8" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="19" t="n">
+      <c r="D8" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="21" t="n">
         <v>32978</v>
       </c>
-      <c r="F8" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>111</v>
+      <c r="F8" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="n">
+      <c r="A9" s="15" t="n">
         <f aca="false">A8+1</f>
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>111</v>
+      <c r="D9" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="n">
+      <c r="A10" s="15" t="n">
         <f aca="false">A9+1</f>
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="19" t="n">
+      <c r="D10" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="21" t="n">
         <v>26992</v>
       </c>
-      <c r="F10" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G10" s="17" t="s">
+      <c r="F10" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>111</v>
+      <c r="H10" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="n">
+      <c r="A11" s="15" t="n">
         <f aca="false">A10+1</f>
         <v>10</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="19" t="n">
+      <c r="C11" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="21" t="n">
         <v>33617</v>
       </c>
-      <c r="F11" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" s="17" t="s">
+      <c r="F11" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>111</v>
+      <c r="H11" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="n">
+      <c r="A12" s="15" t="n">
         <f aca="false">A11+1</f>
         <v>11</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="C12" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17" t="s">
+      <c r="D12" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>111</v>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="n">
+      <c r="A13" s="15" t="n">
         <f aca="false">A12+1</f>
         <v>12</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15" t="n">
+        <f aca="false">A13+1</f>
+        <v>13</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D14" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="17" t="s">
+      <c r="E14" s="21" t="n">
+        <v>38320</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="I13" s="18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="n">
-        <f aca="false">A13+1</f>
-        <v>13</v>
-      </c>
-      <c r="B14" s="14" t="s">
+      <c r="I14" s="20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="n">
+        <f aca="false">A14+1</f>
+        <v>14</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" s="19" t="n">
-        <v>38320</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" s="17" t="s">
+      <c r="C15" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" s="21" t="n">
+        <v>37273</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H15" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="I14" s="18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="n">
-        <f aca="false">A14+1</f>
-        <v>14</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E15" s="19" t="n">
-        <v>37273</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>111</v>
+      <c r="I15" s="20" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="n">
+      <c r="A16" s="15" t="n">
         <f aca="false">A15+1</f>
         <v>15</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17" t="s">
+      <c r="E16" s="19"/>
+      <c r="F16" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="G16" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="I16" s="18" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="n">
+      <c r="A17" s="22" t="n">
         <f aca="false">A16+1</f>
         <v>16</v>
       </c>
-      <c r="B17" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="22" t="s">
+      <c r="B17" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="E17" s="23" t="n">
+      <c r="C17" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="25" t="n">
         <v>33532</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="22" t="s">
+      <c r="G17" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="I17" s="24" t="s">
-        <v>111</v>
+      <c r="I17" s="26" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="10"/>
+      <c r="B18" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18" s="10" t="s">
+      <c r="E18" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="11" t="s">
-        <v>108</v>
+      <c r="I18" s="13" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="25" t="n">
+      <c r="A19" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="28" t="n">
+      <c r="E19" s="30" t="n">
         <v>39970</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" s="29" t="s">
-        <v>114</v>
+      <c r="G19" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="31" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="n">
+      <c r="A20" s="15" t="n">
         <f aca="false">A19+1</f>
         <v>2</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="16" t="n">
+      <c r="E20" s="18" t="n">
         <v>39405</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="18" t="s">
-        <v>115</v>
+      <c r="G20" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13" t="n">
+      <c r="A21" s="15" t="n">
         <f aca="false">A20+1</f>
         <v>3</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="16" t="n">
+      <c r="E21" s="18" t="n">
         <v>39229</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="18" t="s">
-        <v>115</v>
+      <c r="G21" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13" t="n">
+      <c r="A22" s="15" t="n">
         <f aca="false">A21+1</f>
         <v>4</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="16" t="n">
+      <c r="E22" s="18" t="n">
         <v>39179</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="18" t="s">
-        <v>115</v>
+      <c r="G22" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="13" t="n">
+      <c r="A23" s="15" t="n">
         <f aca="false">A22+1</f>
         <v>5</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="16" t="n">
+      <c r="E23" s="18" t="n">
         <v>39514</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="H23" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>115</v>
+      <c r="H23" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13" t="n">
+      <c r="A24" s="15" t="n">
         <f aca="false">A23+1</f>
         <v>6</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="D24" s="15" t="s">
+      <c r="C24" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="18" t="n">
+        <v>39678</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="16" t="n">
-        <v>39678</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13" t="n">
+      <c r="A25" s="15" t="n">
         <f aca="false">A24+1</f>
         <v>7</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="16" t="n">
+      <c r="E25" s="18" t="n">
         <v>39610</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I25" s="18" t="s">
-        <v>115</v>
+      <c r="G25" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="20" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13" t="n">
+      <c r="A26" s="15" t="n">
         <f aca="false">A25+1</f>
         <v>8</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="16" t="n">
+      <c r="E26" s="18" t="n">
         <v>39671</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H26" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I26" s="18" t="s">
-        <v>115</v>
+      <c r="G26" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="13" t="n">
+      <c r="A27" s="15" t="n">
         <f aca="false">A26+1</f>
         <v>9</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="16" t="n">
+      <c r="E27" s="18" t="n">
         <v>38655</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>118</v>
+      <c r="G27" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="13" t="n">
+      <c r="A28" s="15" t="n">
         <f aca="false">A27+1</f>
         <v>10</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="16" t="n">
+      <c r="E28" s="18" t="n">
         <v>38427</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="H28" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I28" s="18" t="s">
-        <v>118</v>
+      <c r="H28" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="20" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="13" t="n">
+      <c r="A29" s="15" t="n">
         <f aca="false">A28+1</f>
         <v>11</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="16" t="n">
+      <c r="E29" s="18" t="n">
         <v>38770</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G29" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H29" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" s="18" t="s">
-        <v>118</v>
+      <c r="G29" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="H29" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="20" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="13" t="n">
+      <c r="A30" s="15" t="n">
         <f aca="false">A29+1</f>
         <v>12</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" s="15" t="s">
+      <c r="C30" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E30" s="16" t="n">
+      <c r="D30" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="18" t="n">
         <v>38099</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G30" s="17" t="s">
+      <c r="G30" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H30" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I30" s="18" t="s">
-        <v>118</v>
+      <c r="H30" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="20" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="13" t="n">
+      <c r="A31" s="15" t="n">
         <f aca="false">A30+1</f>
         <v>13</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E31" s="16" t="n">
+      <c r="E31" s="18" t="n">
         <v>38678</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F31" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G31" s="15" t="s">
+      <c r="G31" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="H31" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I31" s="18" t="s">
-        <v>118</v>
+      <c r="H31" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="20" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="13" t="n">
+      <c r="A32" s="15" t="n">
         <f aca="false">A31+1</f>
         <v>14</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E32" s="16" t="n">
+      <c r="E32" s="18" t="n">
         <v>38919</v>
       </c>
-      <c r="F32" s="15" t="s">
+      <c r="F32" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="15" t="s">
+      <c r="G32" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="H32" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" s="18" t="s">
-        <v>118</v>
+      <c r="H32" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="13" t="n">
+      <c r="A33" s="15" t="n">
         <f aca="false">A32+1</f>
         <v>15</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E33" s="19" t="n">
+      <c r="C33" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" s="21" t="n">
         <v>39400</v>
       </c>
-      <c r="F33" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G33" s="17" t="s">
+      <c r="F33" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="G33" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H33" s="17" t="s">
+      <c r="H33" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="I33" s="18" t="s">
-        <v>115</v>
+      <c r="I33" s="20" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13" t="n">
+      <c r="A34" s="15" t="n">
         <f aca="false">A33+1</f>
         <v>16</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" s="17" t="s">
+      <c r="C34" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="E34" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F34" s="17" t="s">
+      <c r="F34" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="G34" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H34" s="17" t="s">
+      <c r="G34" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="I34" s="18" t="s">
-        <v>115</v>
+      <c r="I34" s="20" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="13" t="n">
+      <c r="A35" s="15" t="n">
         <f aca="false">A34+1</f>
         <v>17</v>
       </c>
-      <c r="B35" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="17" t="s">
+      <c r="B35" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="C35" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="G35" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" s="18" t="s">
-        <v>115</v>
+      <c r="D35" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" s="20" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="20" t="n">
+      <c r="A36" s="22" t="n">
         <f aca="false">A35+1</f>
         <v>18</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E36" s="23" t="n">
+      <c r="E36" s="25" t="n">
         <v>24479</v>
       </c>
-      <c r="F36" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="G36" s="22" t="s">
+      <c r="F36" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="G36" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H36" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="I36" s="24" t="s">
-        <v>115</v>
+      <c r="H36" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="26" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>